<commit_message>
Added rgb variable usage for static color
</commit_message>
<xml_diff>
--- a/info docs/i2c programm IDs.xlsx
+++ b/info docs/i2c programm IDs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="69" documentId="11_AD4DB114E44117BA4C33AC09F950DBF8693EDF2D" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8720FAB8-D49A-4E0C-AC49-EEC7E684C082}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45743734-C5A3-4656-A134-70A766C4E01F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>lila</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>off</t>
+  </si>
+  <si>
+    <t>static color (nach farbauswahl)</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,6 +535,9 @@
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">

</xml_diff>